<commit_message>
vault backup: 2024-10-31 17:14:06
</commit_message>
<xml_diff>
--- a/HandsDatasets/Dataset Summary.xlsx
+++ b/HandsDatasets/Dataset Summary.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Notes\ResearchPapers\HandsDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF89BFE-494B-4463-B89A-F2B5943B4679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933C0EBF-5169-41A1-8CD2-F0E407DF69B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +65,6 @@
     <t>Metadata</t>
   </si>
   <si>
-    <t>Extra notes</t>
-  </si>
-  <si>
     <t>Object mesh</t>
   </si>
   <si>
@@ -423,9 +431,6 @@
     <t>A Dataset of Relighted 3D Interacting Hands</t>
   </si>
   <si>
-    <t>mask</t>
-  </si>
-  <si>
     <t>Meta Reality Lab</t>
   </si>
   <si>
@@ -435,7 +440,73 @@
     <t>Public Scripts</t>
   </si>
   <si>
-    <t>two-hands, address domain gap</t>
+    <t>two-hands, Dynamic render</t>
+  </si>
+  <si>
+    <t>BlurHand</t>
+  </si>
+  <si>
+    <t>Generated from InterHand2.6M</t>
+  </si>
+  <si>
+    <t>No larger than InterHand2.6M</t>
+  </si>
+  <si>
+    <t>Recovering 3D Hand Mesh Sequence from a Single Blurry Image: A New Dataset and Temporal Unfolding</t>
+  </si>
+  <si>
+    <t>Seoul National Univ, Meta Reality</t>
+  </si>
+  <si>
+    <t>https://github.com/JaehaKim97/BlurHand_RELEASE</t>
+  </si>
+  <si>
+    <t>Ego4D</t>
+  </si>
+  <si>
+    <t>Ego4D: Around the World in 3,000 Hours of Egocentric Video</t>
+  </si>
+  <si>
+    <t>Meta, UT Austin, …</t>
+  </si>
+  <si>
+    <t>Egocentric 4D Perception (EGO4D)</t>
+  </si>
+  <si>
+    <t>74 worldwide locations in 9 contries</t>
+  </si>
+  <si>
+    <t>224ego (by different wearers)</t>
+  </si>
+  <si>
+    <t>3.85M sentences of narration</t>
+  </si>
+  <si>
+    <t>Other Related</t>
+  </si>
+  <si>
+    <t>SHOWMe</t>
+  </si>
+  <si>
+    <t>ICCV Workshop</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Scanned object mesh</t>
+  </si>
+  <si>
+    <t>hand mask</t>
+  </si>
+  <si>
+    <t>SHOWMe: Benchmarking Object-agnostic Hand-Object 3D Reconstruction</t>
+  </si>
+  <si>
+    <t>NAVER LABS Europe, Inria centre at Univ Grenoble Alpes</t>
+  </si>
+  <si>
+    <t>SHOWMe - Naver Labs Europe</t>
   </si>
 </sst>
 </file>
@@ -513,7 +584,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -551,22 +622,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -611,6 +671,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -623,26 +692,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -925,92 +985,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="90" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1796875" style="1"/>
+    <col min="14" max="14" width="65.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="77.1796875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.26953125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="1"/>
+    <col min="17" max="17" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="25.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13" t="s">
-        <v>9</v>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="10" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+    <row r="2" spans="1:20" s="10" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>4</v>
@@ -1022,43 +1083,43 @@
         <v>6</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="O2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="S2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="14"/>
+        <v>22</v>
+      </c>
+      <c r="T2" s="17"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2">
         <v>57400000</v>
@@ -1067,60 +1128,60 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="O3" s="1">
         <v>2024</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>14</v>
+      <c r="B4" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="5">
         <v>1500000</v>
@@ -1135,252 +1196,249 @@
         <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1">
         <v>2024</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="T4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>14</v>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="5">
-        <v>1500000</v>
+        <v>87540</v>
       </c>
       <c r="F5" s="1">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="O5" s="1">
         <v>2023</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>64</v>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="F6" s="1">
+        <v>170</v>
+      </c>
+      <c r="G6" s="1">
+        <v>10</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>124</v>
+        <v>21</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="O6" s="1">
         <v>2023</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="13" t="s">
         <v>123</v>
-      </c>
-      <c r="R6" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3030000</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="1">
-        <v>34</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="O7" s="1">
         <v>2023</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A8" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>64</v>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>26712</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>641</v>
-      </c>
+        <f>121839+34057</f>
+        <v>155896</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
@@ -1388,717 +1446,897 @@
       <c r="L8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>67</v>
+      <c r="N8" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="O8" s="1">
         <v>2023</v>
       </c>
       <c r="P8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3030000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1">
+        <v>34</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2">
+        <v>26712</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>641</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="S10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2">
-        <v>230000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="1">
-        <v>12</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="O9" s="1">
-        <v>2022</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2">
-        <v>571645</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="1">
-        <v>4</v>
-      </c>
-      <c r="H10" s="1">
-        <v>8</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="O10" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A11" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="2">
-        <v>103462</v>
-      </c>
-      <c r="F11" s="1">
-        <v>5</v>
+        <v>230000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="G11" s="1">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="O11" s="1">
-        <v>2021</v>
+        <v>2022</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2">
-        <v>582000</v>
-      </c>
-      <c r="F12" s="1">
+        <v>571645</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
         <v>8</v>
       </c>
-      <c r="G12" s="1">
-        <v>10</v>
-      </c>
-      <c r="H12" s="1">
-        <v>20</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="O12" s="1">
         <v>2021</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5">
-        <v>2100000</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>103462</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
       </c>
       <c r="G13" s="1">
         <v>10</v>
       </c>
       <c r="H13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="N13" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="O13" s="1">
         <v>2021</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>125</v>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="2">
+        <v>582000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1">
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2100000</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1">
+        <v>10</v>
+      </c>
+      <c r="H15" s="1">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2">
         <v>2700000</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F16" s="1">
         <v>90</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G16" s="1">
         <v>27</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="O14" s="1">
-        <v>2020</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+      <c r="I16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="R14" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="1">
-        <v>58</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O15" s="1">
-        <v>2020</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2900000</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="1">
-        <v>50</v>
-      </c>
-      <c r="H16" s="1">
-        <v>25</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="O16" s="1">
         <v>2020</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>108</v>
+        <v>127</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="2">
-        <v>77558</v>
-      </c>
-      <c r="F17" s="1">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1">
-        <v>10</v>
-      </c>
       <c r="H17" s="1">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>73</v>
+        <v>20</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="O17" s="1">
         <v>2020</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>75</v>
+        <v>93</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="5">
+        <v>2900000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="1">
+        <v>50</v>
+      </c>
+      <c r="H18" s="1">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O18" s="1">
+        <v>2020</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="2">
+        <v>77558</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10</v>
+      </c>
+      <c r="H19" s="1">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2020</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="5">
         <v>37000</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F20" s="1">
         <v>8</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G20" s="1">
         <v>32</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="8" t="s">
+      <c r="I20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20" s="1">
+        <v>2019</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="1">
+      <c r="R20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2772</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O21" s="1">
         <v>2019</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>71</v>
+      <c r="Q21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="5">
-        <v>21000</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="1">
-        <v>2772</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O19" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>90</v>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2">
+        <v>105459</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="1">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="2">
-        <v>105459</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="1">
-        <v>6</v>
-      </c>
-      <c r="H20" s="1">
-        <v>4</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="O20" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>42</v>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" s="1">
+        <v>931</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4336</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:M1"/>
@@ -2111,24 +2349,27 @@
   <hyperlinks>
     <hyperlink ref="R3" r:id="rId1" location="both57m-dataset" xr:uid="{6093CB3F-7559-4A60-9533-FC5A6593C8DF}"/>
     <hyperlink ref="R4" r:id="rId2" display="https://hograspnet2024.github.io/" xr:uid="{DF9465E4-05AF-4DCB-BCDC-1DC144B7533F}"/>
-    <hyperlink ref="R13" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
-    <hyperlink ref="R7" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
-    <hyperlink ref="R12" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
-    <hyperlink ref="R8" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
-    <hyperlink ref="R17" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
-    <hyperlink ref="R11" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
-    <hyperlink ref="R18" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
-    <hyperlink ref="R19" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
-    <hyperlink ref="R15" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
-    <hyperlink ref="R20" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
-    <hyperlink ref="R16" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
-    <hyperlink ref="R10" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
-    <hyperlink ref="R9" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
-    <hyperlink ref="R6" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
-    <hyperlink ref="R14" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
-    <hyperlink ref="R5" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
+    <hyperlink ref="R15" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
+    <hyperlink ref="R9" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
+    <hyperlink ref="R14" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
+    <hyperlink ref="R10" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
+    <hyperlink ref="R19" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
+    <hyperlink ref="R13" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
+    <hyperlink ref="R20" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
+    <hyperlink ref="R21" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
+    <hyperlink ref="R17" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
+    <hyperlink ref="R22" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
+    <hyperlink ref="R18" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
+    <hyperlink ref="R12" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
+    <hyperlink ref="R11" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
+    <hyperlink ref="R7" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
+    <hyperlink ref="R16" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
+    <hyperlink ref="R6" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
+    <hyperlink ref="R8" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
+    <hyperlink ref="R25" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
+    <hyperlink ref="R5" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2024-11-18 11:03:47
</commit_message>
<xml_diff>
--- a/HandsDatasets/Dataset Summary.xlsx
+++ b/HandsDatasets/Dataset Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Notes\ResearchPapers\HandsDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933C0EBF-5169-41A1-8CD2-F0E407DF69B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EDC60-444F-48B0-9C5A-8A95AE79B1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="173">
   <si>
     <t>Name</t>
   </si>
@@ -446,9 +446,6 @@
     <t>BlurHand</t>
   </si>
   <si>
-    <t>Generated from InterHand2.6M</t>
-  </si>
-  <si>
     <t>No larger than InterHand2.6M</t>
   </si>
   <si>
@@ -507,6 +504,57 @@
   </si>
   <si>
     <t>SHOWMe - Naver Labs Europe</t>
+  </si>
+  <si>
+    <t>COMIC</t>
+  </si>
+  <si>
+    <t>Object Category</t>
+  </si>
+  <si>
+    <t>CHORD : Category-level Hand-held Object Reconstruction via Shape Deformatio</t>
+  </si>
+  <si>
+    <t>SJTU, Shanghai Qi Zhi Institute, South China Univ of Tech, XREAL</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/LiKailin/COMIC/tree/main/comic</t>
+  </si>
+  <si>
+    <t>Dataloader will be released soon</t>
+  </si>
+  <si>
+    <t>6 categories from OakInk</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> InterHand2.6M</t>
+  </si>
+  <si>
+    <t>HO3Dv2</t>
+  </si>
+  <si>
+    <t>HMDO</t>
+  </si>
+  <si>
+    <t>Object Deformation map</t>
+  </si>
+  <si>
+    <t>HMDO : Markerless multi-view hand manipulation capture with deformable objects</t>
+  </si>
+  <si>
+    <t>Graphical Models</t>
+  </si>
+  <si>
+    <t>Southeast Univ</t>
+  </si>
+  <si>
+    <t>https://github.com/WeiXie-wx/HMDO</t>
+  </si>
+  <si>
+    <t>BaiduNetDisk</t>
   </si>
 </sst>
 </file>
@@ -635,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,29 +728,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -985,13 +1030,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1002,65 +1047,69 @@
     <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="65.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="18.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="25.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="1" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16" t="s">
-        <v>151</v>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="10" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+    <row r="2" spans="1:21" s="10" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
@@ -1106,13 +1155,14 @@
       <c r="S2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="17"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1170,11 +1220,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1232,30 +1282,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="5">
-        <v>87540</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21600</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>20</v>
@@ -1269,34 +1316,34 @@
       <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="8" t="s">
-        <v>154</v>
+      <c r="M5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="O5" s="1">
         <v>2023</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="R5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>13</v>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -1304,17 +1351,14 @@
       <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5">
-        <v>1500000</v>
+      <c r="E6" s="2">
+        <v>426000</v>
       </c>
       <c r="F6" s="1">
-        <v>170</v>
-      </c>
-      <c r="G6" s="1">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
@@ -1323,60 +1367,63 @@
         <v>20</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>130</v>
+        <v>157</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="O6" s="1">
         <v>2023</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>63</v>
+        <v>148</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="E7" s="5">
+        <v>87540</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>15</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>20</v>
@@ -1385,38 +1432,38 @@
         <v>20</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>123</v>
+        <v>20</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="O7" s="1">
         <v>2023</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>121</v>
+        <v>154</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1425,250 +1472,253 @@
       <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="F8" s="1">
+        <v>170</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
         <f>121839+34057</f>
         <v>155896</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F10" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="O8" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="R8" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="2">
-        <v>3030000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1">
-        <v>34</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="2">
-        <v>26712</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>641</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="O10" s="1">
         <v>2023</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>69</v>
+        <v>138</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2">
-        <v>230000</v>
+        <v>3030000</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="O11" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2">
-        <v>571645</v>
+        <v>26712</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>8</v>
+        <v>641</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>20</v>
@@ -1682,84 +1732,90 @@
       <c r="L12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="23" t="s">
-        <v>108</v>
+      <c r="M12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="O12" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>67</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2">
-        <v>103462</v>
-      </c>
-      <c r="F13" s="1">
-        <v>5</v>
+        <v>230000</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="G13" s="1">
-        <v>10</v>
-      </c>
-      <c r="H13" s="1">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="O13" s="1">
-        <v>2021</v>
+        <v>2022</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1771,17 +1827,17 @@
         <v>27</v>
       </c>
       <c r="E14" s="2">
-        <v>582000</v>
-      </c>
-      <c r="F14" s="1">
+        <v>571645</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1">
         <v>8</v>
       </c>
-      <c r="G14" s="1">
-        <v>10</v>
-      </c>
-      <c r="H14" s="1">
-        <v>20</v>
-      </c>
       <c r="I14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1794,28 +1850,28 @@
       <c r="L14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="8" t="s">
-        <v>59</v>
+      <c r="N14" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="O14" s="1">
         <v>2021</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1826,58 +1882,55 @@
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="5">
-        <v>2100000</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
+      <c r="E15" s="2">
+        <v>103462</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
       </c>
       <c r="G15" s="1">
         <v>10</v>
       </c>
       <c r="H15" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="O15" s="1">
         <v>2021</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>45</v>
+        <v>119</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1886,75 +1939,75 @@
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
+        <v>582000</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="2">
-        <v>2700000</v>
-      </c>
-      <c r="F16" s="1">
-        <v>90</v>
-      </c>
-      <c r="G16" s="1">
-        <v>27</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="O16" s="1">
-        <v>2020</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R16" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>97</v>
+      <c r="E17" s="5">
+        <v>2100000</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="G17" s="1">
+        <v>10</v>
       </c>
       <c r="H17" s="1">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>20</v>
@@ -1963,36 +2016,39 @@
         <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>92</v>
+        <v>44</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="O17" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>91</v>
+        <v>47</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -2001,37 +2057,34 @@
         <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2700000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>90</v>
+      </c>
+      <c r="G18" s="1">
         <v>27</v>
       </c>
-      <c r="E18" s="5">
-        <v>2900000</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" s="1">
-        <v>50</v>
-      </c>
       <c r="H18" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="O18" s="1">
         <v>2020</v>
@@ -2040,66 +2093,69 @@
         <v>39</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>107</v>
+        <v>127</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="2">
-        <v>77558</v>
-      </c>
-      <c r="F19" s="1">
-        <v>5</v>
-      </c>
-      <c r="G19" s="1">
-        <v>10</v>
+        <v>95</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H19" s="1">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>72</v>
+        <v>20</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="O19" s="1">
         <v>2020</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>74</v>
+        <v>93</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>70</v>
@@ -2107,7 +2163,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2116,19 +2172,19 @@
         <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" s="5">
-        <v>37000</v>
-      </c>
-      <c r="F20" s="1">
-        <v>8</v>
+        <v>2900000</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G20" s="1">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>20</v>
@@ -2137,25 +2193,28 @@
         <v>20</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="O20" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>70</v>
@@ -2163,180 +2222,293 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="5">
-        <v>21000</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E21" s="2">
+        <v>77558</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>10</v>
       </c>
       <c r="H21" s="1">
-        <v>2772</v>
+        <v>10</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="O21" s="1">
-        <v>2019</v>
+        <v>2020</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="5">
+        <v>37000</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1">
+        <v>32</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="L22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2019</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2772</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E24" s="2">
         <v>105459</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G24" s="1">
         <v>6</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H24" s="1">
         <v>4</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="I24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="1" t="s">
+      <c r="K24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N22" s="13" t="s">
+      <c r="N24" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O24" s="1">
         <v>2018</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R22" s="7" t="s">
+      <c r="R24" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>148</v>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" s="1">
+        <v>931</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4336</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G25" s="1">
-        <v>931</v>
-      </c>
-      <c r="H25" s="1">
-        <v>4336</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N25" s="8" t="s">
+      <c r="O27" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O25" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R27" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="R25" s="6" t="s">
+      <c r="T27" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="F8:H8"/>
+  <mergeCells count="10">
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:M1"/>
@@ -2349,27 +2521,28 @@
   <hyperlinks>
     <hyperlink ref="R3" r:id="rId1" location="both57m-dataset" xr:uid="{6093CB3F-7559-4A60-9533-FC5A6593C8DF}"/>
     <hyperlink ref="R4" r:id="rId2" display="https://hograspnet2024.github.io/" xr:uid="{DF9465E4-05AF-4DCB-BCDC-1DC144B7533F}"/>
-    <hyperlink ref="R15" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
-    <hyperlink ref="R9" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
-    <hyperlink ref="R14" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
-    <hyperlink ref="R10" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
-    <hyperlink ref="R19" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
-    <hyperlink ref="R13" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
-    <hyperlink ref="R20" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
-    <hyperlink ref="R21" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
-    <hyperlink ref="R17" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
-    <hyperlink ref="R22" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
-    <hyperlink ref="R18" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
-    <hyperlink ref="R12" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
-    <hyperlink ref="R11" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
-    <hyperlink ref="R7" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
-    <hyperlink ref="R16" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
-    <hyperlink ref="R6" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
-    <hyperlink ref="R8" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
-    <hyperlink ref="R25" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
-    <hyperlink ref="R5" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
+    <hyperlink ref="R17" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
+    <hyperlink ref="R11" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
+    <hyperlink ref="R16" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
+    <hyperlink ref="R12" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
+    <hyperlink ref="R21" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
+    <hyperlink ref="R15" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
+    <hyperlink ref="R22" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
+    <hyperlink ref="R23" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
+    <hyperlink ref="R19" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
+    <hyperlink ref="R24" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
+    <hyperlink ref="R20" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
+    <hyperlink ref="R14" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
+    <hyperlink ref="R13" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
+    <hyperlink ref="R9" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
+    <hyperlink ref="R18" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
+    <hyperlink ref="R8" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
+    <hyperlink ref="R10" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
+    <hyperlink ref="R27" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
+    <hyperlink ref="R7" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
+    <hyperlink ref="R6" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2024-11-26 17:54:32
</commit_message>
<xml_diff>
--- a/HandsDatasets/Dataset Summary.xlsx
+++ b/HandsDatasets/Dataset Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Notes\ResearchPapers\HandsDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EDC60-444F-48B0-9C5A-8A95AE79B1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24BE02-2AA2-4C6A-A7A6-AE83B7C32410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9480" yWindow="3780" windowWidth="18820" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
   <si>
     <t>Name</t>
   </si>
@@ -555,6 +555,24 @@
   </si>
   <si>
     <t>BaiduNetDisk</t>
+  </si>
+  <si>
+    <t>HanCo</t>
+  </si>
+  <si>
+    <t>University of Freiburg</t>
+  </si>
+  <si>
+    <t>PGCV</t>
+  </si>
+  <si>
+    <t>Hand / forearm mask</t>
+  </si>
+  <si>
+    <t>Contrastive Representation Learning for Hand Shape Estimation</t>
+  </si>
+  <si>
+    <t>The first hand dataset with synchronized multi-view frames; captured with green mask so we can randomize the background.</t>
   </si>
 </sst>
 </file>
@@ -683,7 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -700,7 +718,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -720,12 +737,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -749,6 +760,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,139 +1043,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="14" max="14" width="38.453125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7265625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="14" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="10" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="11" t="s">
+    <row r="2" spans="1:21" s="9" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="19"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1220,8 +1233,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1272,7 +1285,7 @@
       <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -1282,8 +1295,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" s="11" t="s">
         <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1331,15 +1344,15 @@
       <c r="Q5" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="6" t="s">
         <v>171</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
         <v>156</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1387,7 +1400,7 @@
       <c r="Q6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="20" t="s">
         <v>160</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -1400,8 +1413,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A7" s="11" t="s">
         <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1437,7 +1450,7 @@
       <c r="L7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="7" t="s">
         <v>153</v>
       </c>
       <c r="O7" s="1">
@@ -1449,7 +1462,7 @@
       <c r="Q7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="20" t="s">
         <v>155</v>
       </c>
       <c r="S7" s="1" t="s">
@@ -1459,8 +1472,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1499,7 +1512,7 @@
       <c r="M8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="7" t="s">
         <v>130</v>
       </c>
       <c r="O8" s="1">
@@ -1511,7 +1524,7 @@
       <c r="Q8" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="20" t="s">
         <v>132</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1521,8 +1534,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A9" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1558,7 +1571,7 @@
       <c r="L9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="12" t="s">
         <v>123</v>
       </c>
       <c r="O9" s="1">
@@ -1570,7 +1583,7 @@
       <c r="Q9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="3" t="s">
         <v>121</v>
       </c>
       <c r="S9" s="1" t="s">
@@ -1580,8 +1593,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A10" s="11" t="s">
         <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1597,11 +1610,11 @@
         <f>121839+34057</f>
         <v>155896</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1614,7 +1627,7 @@
       <c r="L10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="13" t="s">
+      <c r="N10" s="12" t="s">
         <v>137</v>
       </c>
       <c r="O10" s="1">
@@ -1626,7 +1639,7 @@
       <c r="Q10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="3" t="s">
         <v>139</v>
       </c>
       <c r="S10" s="1" t="s">
@@ -1636,8 +1649,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1673,7 +1686,7 @@
       <c r="L11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="7" t="s">
         <v>51</v>
       </c>
       <c r="O11" s="1">
@@ -1685,7 +1698,7 @@
       <c r="Q11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="S11" s="1" t="s">
@@ -1695,8 +1708,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1735,7 +1748,7 @@
       <c r="M12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="7" t="s">
         <v>66</v>
       </c>
       <c r="O12" s="1">
@@ -1747,15 +1760,15 @@
       <c r="Q12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R12" s="7" t="s">
+      <c r="R12" s="6" t="s">
         <v>69</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1794,7 +1807,7 @@
       <c r="M13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>114</v>
       </c>
       <c r="O13" s="1">
@@ -1806,15 +1819,15 @@
       <c r="Q13" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="6" t="s">
         <v>118</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1850,7 +1863,7 @@
       <c r="L14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="14" t="s">
         <v>108</v>
       </c>
       <c r="O14" s="1">
@@ -1862,15 +1875,15 @@
       <c r="Q14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="R14" s="7" t="s">
+      <c r="R14" s="6" t="s">
         <v>110</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1906,7 +1919,7 @@
       <c r="L15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="7" t="s">
         <v>76</v>
       </c>
       <c r="O15" s="1">
@@ -1915,7 +1928,7 @@
       <c r="Q15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R15" s="7" t="s">
+      <c r="R15" s="6" t="s">
         <v>74</v>
       </c>
       <c r="S15" s="1" t="s">
@@ -1928,8 +1941,8 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1965,7 +1978,7 @@
       <c r="L16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="7" t="s">
         <v>59</v>
       </c>
       <c r="O16" s="1">
@@ -1977,15 +1990,15 @@
       <c r="Q16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R16" s="7" t="s">
+      <c r="R16" s="6" t="s">
         <v>61</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2024,7 +2037,7 @@
       <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N17" s="7" t="s">
         <v>46</v>
       </c>
       <c r="O17" s="1">
@@ -2036,7 +2049,7 @@
       <c r="Q17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="7" t="s">
+      <c r="R17" s="6" t="s">
         <v>42</v>
       </c>
       <c r="S17" s="1" t="s">
@@ -2046,9 +2059,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>124</v>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A18" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -2059,14 +2072,11 @@
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2">
-        <v>2700000</v>
+      <c r="E18" s="5">
+        <v>860304</v>
       </c>
       <c r="F18" s="1">
-        <v>90</v>
-      </c>
-      <c r="G18" s="1">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -2075,7 +2085,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>21</v>
@@ -2083,108 +2093,111 @@
       <c r="L18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="8" t="s">
-        <v>128</v>
+      <c r="M18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="O18" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R18" s="15" t="s">
-        <v>129</v>
+        <v>175</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="T18" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>81</v>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2700000</v>
+      </c>
+      <c r="F19" s="1">
+        <v>90</v>
+      </c>
+      <c r="G19" s="1">
+        <v>27</v>
       </c>
       <c r="H19" s="1">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>92</v>
+        <v>21</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="O19" s="1">
         <v>2020</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>91</v>
+        <v>127</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>83</v>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="5">
-        <v>2900000</v>
+        <v>95</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="1">
-        <v>50</v>
+        <v>98</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H20" s="1">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>20</v>
@@ -2193,36 +2206,36 @@
         <v>20</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>106</v>
+        <v>35</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="O20" s="1">
         <v>2020</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>71</v>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -2231,54 +2244,57 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="2">
-        <v>77558</v>
-      </c>
-      <c r="F21" s="1">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2900000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G21" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H21" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>72</v>
+        <v>20</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="O21" s="1">
         <v>2020</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>74</v>
+        <v>104</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>58</v>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
@@ -2289,73 +2305,73 @@
       <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="5">
-        <v>37000</v>
+      <c r="E22" s="2">
+        <v>77558</v>
       </c>
       <c r="F22" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G22" s="1">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N22" s="8" t="s">
-        <v>77</v>
+      <c r="N22" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="O22" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>80</v>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A23" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="E23" s="5">
-        <v>21000</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>14</v>
+        <v>37000</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1">
+        <v>32</v>
       </c>
       <c r="H23" s="1">
-        <v>2772</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>20</v>
@@ -2364,144 +2380,200 @@
         <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="O23" s="1">
         <v>2019</v>
       </c>
+      <c r="P23" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="Q23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2772</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="R24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A25" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>105459</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G25" s="1">
         <v>6</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H25" s="1">
         <v>4</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="1" t="s">
+      <c r="I25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N24" s="13" t="s">
+      <c r="N25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O25" s="1">
         <v>2018</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R24" s="7" t="s">
+      <c r="R25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G28" s="1">
         <v>931</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H28" s="1">
         <v>4336</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M27" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="N27" s="8" t="s">
+      <c r="N28" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O28" s="1">
         <v>2021</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="R27" s="6" t="s">
+      <c r="R28" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="T27" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2525,24 +2597,25 @@
     <hyperlink ref="R11" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
     <hyperlink ref="R16" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
     <hyperlink ref="R12" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
-    <hyperlink ref="R21" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
+    <hyperlink ref="R22" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
     <hyperlink ref="R15" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
-    <hyperlink ref="R22" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
-    <hyperlink ref="R23" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
-    <hyperlink ref="R19" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
-    <hyperlink ref="R24" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
-    <hyperlink ref="R20" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
+    <hyperlink ref="R23" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
+    <hyperlink ref="R24" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
+    <hyperlink ref="R20" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
+    <hyperlink ref="R25" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
+    <hyperlink ref="R21" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
     <hyperlink ref="R14" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
     <hyperlink ref="R13" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
     <hyperlink ref="R9" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
-    <hyperlink ref="R18" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
+    <hyperlink ref="R19" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
     <hyperlink ref="R8" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
     <hyperlink ref="R10" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
-    <hyperlink ref="R27" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
+    <hyperlink ref="R28" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
     <hyperlink ref="R7" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
     <hyperlink ref="R6" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
+    <hyperlink ref="R18" r:id="rId23" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/HanCo.en.html" xr:uid="{1D766960-F6F8-4DD4-BE6E-EE217414AB48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2024-12-05 21:10:21
</commit_message>
<xml_diff>
--- a/HandsDatasets/Dataset Summary.xlsx
+++ b/HandsDatasets/Dataset Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Notes\ResearchPapers\HandsDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24BE02-2AA2-4C6A-A7A6-AE83B7C32410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EB168B-B121-4E85-A00D-BFF86DAF8750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="3780" windowWidth="18820" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -350,9 +350,6 @@
     <t>guiggh/hand_pose_action: Dataset and code for the paper "First-Person Hand Action Benchmark with RGB-D Videos and 3D Hand Pose Annotations", CVPR 2018.</t>
   </si>
   <si>
-    <t>Georgia Tech, Facebook Reality</t>
-  </si>
-  <si>
     <t>Contact Map</t>
   </si>
   <si>
@@ -573,6 +570,60 @@
   </si>
   <si>
     <t>The first hand dataset with synchronized multi-view frames; captured with green mask so we can randomize the background.</t>
+  </si>
+  <si>
+    <t>HOH</t>
+  </si>
+  <si>
+    <t>HOH: Markerless Multimodal Human-Object-Human Handover Dataset with Large Object Count</t>
+  </si>
+  <si>
+    <t>Clarkson Univ</t>
+  </si>
+  <si>
+    <t>HOH: Human-Object-Human Handover</t>
+  </si>
+  <si>
+    <t>Email Authors</t>
+  </si>
+  <si>
+    <t>AIH</t>
+  </si>
+  <si>
+    <t>3D Interacting Hand Pose Estimation by Hand De-occlusion and Removal</t>
+  </si>
+  <si>
+    <t>HDR</t>
+  </si>
+  <si>
+    <t>amodal hand segmentation</t>
+  </si>
+  <si>
+    <t>two-hands(AIH_Syn + AIH_Render)</t>
+  </si>
+  <si>
+    <t>PressureVisionDB</t>
+  </si>
+  <si>
+    <t>Georgia Tech, Intel, Meta Reality</t>
+  </si>
+  <si>
+    <t>Georgia Tech, Intel, Facebook Reality</t>
+  </si>
+  <si>
+    <t>https://github.com/facebookresearch/PressureVision</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>w/ a pressure sensor</t>
+  </si>
+  <si>
+    <t>PressureVision: Estimating Hand Pressure from a Single RGB Image</t>
+  </si>
+  <si>
+    <t>Contact Pressure</t>
   </si>
 </sst>
 </file>
@@ -701,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,6 +796,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,8 +814,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1043,13 +1095,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -1067,7 +1119,7 @@
     <col min="11" max="11" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7265625" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="41.1796875" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.1796875" style="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
@@ -1078,51 +1130,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>163</v>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="9" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
@@ -1168,8 +1220,8 @@
       <c r="S2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -1297,7 +1349,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1305,58 +1357,32 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2">
-        <v>21600</v>
-      </c>
-      <c r="F5" s="1">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>168</v>
+      <c r="E5" s="5"/>
+      <c r="N5" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="O5" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>171</v>
+        <v>180</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -1365,13 +1391,13 @@
         <v>26</v>
       </c>
       <c r="E6" s="2">
-        <v>426000</v>
+        <v>21600</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>162</v>
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
@@ -1386,57 +1412,48 @@
         <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="O6" s="1">
         <v>2023</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>160</v>
+        <v>169</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="5">
-        <v>87540</v>
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>426000</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1">
-        <v>42</v>
+      <c r="H7" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>20</v>
@@ -1450,31 +1467,37 @@
       <c r="L7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>153</v>
+      <c r="M7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="O7" s="1">
         <v>2023</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>149</v>
+        <v>67</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="R7" s="20" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>70</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>151</v>
+        <v>160</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1483,19 +1506,19 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5">
-        <v>1500000</v>
+        <v>87540</v>
       </c>
       <c r="F8" s="1">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
@@ -1504,57 +1527,54 @@
         <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="O8" s="1">
         <v>2023</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>132</v>
+        <v>153</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>170</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -1571,123 +1591,126 @@
       <c r="L9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="12" t="s">
-        <v>123</v>
+      <c r="M9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="O9" s="1">
         <v>2023</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>121</v>
+        <v>130</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <f>121839+34057</f>
         <v>155896</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F11" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="O10" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3030000</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="1">
-        <v>34</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="O11" s="1">
         <v>2023</v>
@@ -1696,254 +1719,254 @@
         <v>16</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>53</v>
+        <v>137</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>55</v>
+      <c r="U11" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2">
-        <v>26712</v>
+        <v>3030000</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>641</v>
-      </c>
       <c r="I12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="O12" s="1">
         <v>2023</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2">
+        <v>26712</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>641</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="G14" s="1">
         <v>27</v>
       </c>
-      <c r="E13" s="2">
-        <v>230000</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="1">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="O13" s="1">
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="O14" s="1">
         <v>2022</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="2">
-        <v>571645</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G14" s="1">
-        <v>4</v>
-      </c>
-      <c r="H14" s="1">
-        <v>8</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="O14" s="1">
-        <v>2021</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>110</v>
+        <v>39</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2">
-        <v>103462</v>
-      </c>
-      <c r="F15" s="1">
-        <v>5</v>
+        <v>230000</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G15" s="1">
-        <v>10</v>
-      </c>
-      <c r="H15" s="1">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="O15" s="1">
-        <v>2021</v>
+        <v>2022</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1955,17 +1978,17 @@
         <v>27</v>
       </c>
       <c r="E16" s="2">
-        <v>582000</v>
-      </c>
-      <c r="F16" s="1">
+        <v>571645</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
         <v>8</v>
       </c>
-      <c r="G16" s="1">
-        <v>10</v>
-      </c>
-      <c r="H16" s="1">
-        <v>20</v>
-      </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1978,28 +2001,28 @@
       <c r="L16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="7" t="s">
-        <v>59</v>
+      <c r="N16" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="O16" s="1">
         <v>2021</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -2010,58 +2033,55 @@
       <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="5">
-        <v>2100000</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>43</v>
+      <c r="E17" s="2">
+        <v>103462</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5</v>
       </c>
       <c r="G17" s="1">
         <v>10</v>
       </c>
       <c r="H17" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="O17" s="1">
         <v>2021</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -2070,16 +2090,19 @@
         <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="5">
-        <v>860304</v>
+        <v>27</v>
+      </c>
+      <c r="E18" s="2">
+        <v>582000</v>
       </c>
       <c r="F18" s="1">
         <v>8</v>
       </c>
+      <c r="G18" s="1">
+        <v>10</v>
+      </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>20</v>
@@ -2088,39 +2111,33 @@
         <v>20</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N18" s="21" t="s">
-        <v>177</v>
+        <v>20</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="O18" s="1">
         <v>2021</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q18" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="R18" s="20" t="s">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -2131,74 +2148,77 @@
       <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2">
-        <v>2700000</v>
-      </c>
-      <c r="F19" s="1">
-        <v>90</v>
+      <c r="E19" s="5">
+        <v>2100000</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G19" s="1">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="H19" s="1">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="5">
+        <v>860304</v>
+      </c>
+      <c r="F20" s="1">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="O19" s="1">
-        <v>2020</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1">
-        <v>58</v>
-      </c>
       <c r="I20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2206,36 +2226,39 @@
         <v>20</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>92</v>
+        <v>175</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="O20" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>91</v>
+        <v>174</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="T20" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -2244,37 +2267,34 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2700000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>90</v>
+      </c>
+      <c r="G21" s="1">
         <v>27</v>
       </c>
-      <c r="E21" s="5">
-        <v>2900000</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="1">
-        <v>50</v>
-      </c>
       <c r="H21" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="O21" s="1">
         <v>2020</v>
@@ -2283,74 +2303,77 @@
         <v>39</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="2">
-        <v>77558</v>
-      </c>
-      <c r="F22" s="1">
-        <v>5</v>
-      </c>
-      <c r="G22" s="1">
-        <v>10</v>
+        <v>95</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H22" s="1">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>72</v>
+        <v>20</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="O22" s="1">
         <v>2020</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>74</v>
+        <v>93</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -2359,19 +2382,19 @@
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" s="5">
-        <v>37000</v>
-      </c>
-      <c r="F23" s="1">
-        <v>8</v>
+        <v>2900000</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="G23" s="1">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>20</v>
@@ -2380,207 +2403,385 @@
         <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="O23" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="5">
-        <v>21000</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E24" s="2">
+        <v>77558</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>10</v>
       </c>
       <c r="H24" s="1">
-        <v>2772</v>
+        <v>10</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="O24" s="1">
-        <v>2019</v>
+        <v>2020</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="5">
+        <v>37000</v>
+      </c>
+      <c r="F25" s="1">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1">
+        <v>32</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A26" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2772</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O26" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E27" s="2">
         <v>105459</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G27" s="1">
         <v>6</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H27" s="1">
         <v>4</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="1" t="s">
+      <c r="I27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N25" s="12" t="s">
+      <c r="N27" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O27" s="1">
         <v>2018</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R25" s="6" t="s">
+      <c r="R27" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A30" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="2">
+        <f>490000*6</f>
+        <v>2940000</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>36</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2022</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="1">
+        <v>931</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4336</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" s="1">
-        <v>931</v>
-      </c>
-      <c r="H28" s="1">
-        <v>4336</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="N28" s="7" t="s">
+      <c r="O31" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="O28" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q28" s="1" t="s">
+      <c r="R31" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="R28" s="20" t="s">
+      <c r="T31" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:M1"/>
@@ -2593,29 +2794,31 @@
   <hyperlinks>
     <hyperlink ref="R3" r:id="rId1" location="both57m-dataset" xr:uid="{6093CB3F-7559-4A60-9533-FC5A6593C8DF}"/>
     <hyperlink ref="R4" r:id="rId2" display="https://hograspnet2024.github.io/" xr:uid="{DF9465E4-05AF-4DCB-BCDC-1DC144B7533F}"/>
-    <hyperlink ref="R17" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
-    <hyperlink ref="R11" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
-    <hyperlink ref="R16" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
-    <hyperlink ref="R12" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
-    <hyperlink ref="R22" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
-    <hyperlink ref="R15" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
-    <hyperlink ref="R23" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
-    <hyperlink ref="R24" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
-    <hyperlink ref="R20" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
-    <hyperlink ref="R25" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
-    <hyperlink ref="R21" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
-    <hyperlink ref="R14" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
-    <hyperlink ref="R13" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
-    <hyperlink ref="R9" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
-    <hyperlink ref="R19" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
-    <hyperlink ref="R8" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
-    <hyperlink ref="R10" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
-    <hyperlink ref="R28" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
-    <hyperlink ref="R7" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
-    <hyperlink ref="R6" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
-    <hyperlink ref="R18" r:id="rId23" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/HanCo.en.html" xr:uid="{1D766960-F6F8-4DD4-BE6E-EE217414AB48}"/>
+    <hyperlink ref="R19" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
+    <hyperlink ref="R12" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
+    <hyperlink ref="R18" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
+    <hyperlink ref="R13" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
+    <hyperlink ref="R24" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
+    <hyperlink ref="R17" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
+    <hyperlink ref="R25" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
+    <hyperlink ref="R26" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
+    <hyperlink ref="R22" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
+    <hyperlink ref="R27" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
+    <hyperlink ref="R23" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
+    <hyperlink ref="R16" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
+    <hyperlink ref="R15" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
+    <hyperlink ref="R10" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
+    <hyperlink ref="R21" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
+    <hyperlink ref="R9" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
+    <hyperlink ref="R11" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
+    <hyperlink ref="R31" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
+    <hyperlink ref="R8" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
+    <hyperlink ref="R7" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
+    <hyperlink ref="R20" r:id="rId23" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/HanCo.en.html" xr:uid="{1D766960-F6F8-4DD4-BE6E-EE217414AB48}"/>
+    <hyperlink ref="R5" r:id="rId24" display="https://tars-home.github.io/hohdataset/" xr:uid="{9D883F19-E811-4E4A-8132-DA3D28491038}"/>
+    <hyperlink ref="R14" r:id="rId25" display="https://menghao666.github.io/HDR/" xr:uid="{CC6BDE28-D08F-4D4E-BC32-67420002F467}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-06-10 11:23:40
</commit_message>
<xml_diff>
--- a/HandsDatasets/Dataset Summary.xlsx
+++ b/HandsDatasets/Dataset Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Notes\ResearchPapers\HandsDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EB168B-B121-4E85-A00D-BFF86DAF8750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D402FD-5AAF-49BE-ACFC-6D440EF0CDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4150" yWindow="3190" windowWidth="21580" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -624,6 +624,70 @@
   </si>
   <si>
     <t>Contact Pressure</t>
+  </si>
+  <si>
+    <t>OakInk2</t>
+  </si>
+  <si>
+    <t>OAKINK2 : A Dataset of Bimanual Hands-Object Manipulation
+in Complex Task Completion</t>
+  </si>
+  <si>
+    <t>SJTU, South China Univ of Tech</t>
+  </si>
+  <si>
+    <t>3+1ego</t>
+  </si>
+  <si>
+    <t>OAKINK2 Dataset CVPR2024 | 双手复杂任务操作</t>
+  </si>
+  <si>
+    <t>Two-hands object manipulation</t>
+  </si>
+  <si>
+    <t>two hands manipulation; bimanual</t>
+  </si>
+  <si>
+    <t>TACO</t>
+  </si>
+  <si>
+    <t>RGB (D for ego)</t>
+  </si>
+  <si>
+    <t>12 + 1ego</t>
+  </si>
+  <si>
+    <t>tool category, action label, target object category</t>
+  </si>
+  <si>
+    <t>TACO: Benchmarking Generalizable Bimanual Tool-ACtion-Object Understanding</t>
+  </si>
+  <si>
+    <t>Tsinghua Univ, Shanghai AI Lab, Shanghai Qi Zhi Institute, Beijing U of P &amp; T, Beijing Institute of Tech</t>
+  </si>
+  <si>
+    <t>Dropbox</t>
+  </si>
+  <si>
+    <t>HOI4D</t>
+  </si>
+  <si>
+    <t>HOI4D: A 4D Egocentric Dataset for Category-Level Human-Object Interaction</t>
+  </si>
+  <si>
+    <t>GRAB</t>
+  </si>
+  <si>
+    <t>GRAB: A Dataset of Whole-Body Human Grasping of Objects</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>Register an Account</t>
+  </si>
+  <si>
+    <t>Body Model; contact info</t>
   </si>
 </sst>
 </file>
@@ -1095,13 +1159,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -1123,7 +1187,7 @@
     <col min="15" max="15" width="9.1796875" style="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="44.26953125" style="1" customWidth="1"/>
     <col min="19" max="19" width="18.81640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="14" style="1" customWidth="1"/>
     <col min="21" max="16384" width="9.1796875" style="1"/>
@@ -1347,9 +1411,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1357,29 +1421,58 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="N5" s="16" t="s">
-        <v>179</v>
+      <c r="D5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5200000</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G5" s="1">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1">
+        <v>196</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="O5" s="1">
         <v>2024</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>181</v>
+        <v>208</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>207</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1391,13 +1484,16 @@
         <v>26</v>
       </c>
       <c r="E6" s="2">
-        <v>21600</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10</v>
+        <v>4010000</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9</v>
       </c>
       <c r="H6" s="1">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
@@ -1412,92 +1508,63 @@
         <v>20</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="O6" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>168</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>170</v>
+        <v>198</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>200</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>171</v>
+        <v>70</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2">
-        <v>426000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>157</v>
+      <c r="E7" s="5"/>
+      <c r="N7" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="O7" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1509,16 +1576,16 @@
         <v>27</v>
       </c>
       <c r="E8" s="5">
-        <v>87540</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
+        <v>2100000</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G8" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
@@ -1532,31 +1599,34 @@
       <c r="L8" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="M8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="N8" s="7" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="O8" s="1">
         <v>2023</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>154</v>
+        <v>47</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
@@ -1567,17 +1637,14 @@
       <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="5">
-        <v>1500000</v>
+      <c r="E9" s="2">
+        <v>21600</v>
       </c>
       <c r="F9" s="1">
-        <v>170</v>
-      </c>
-      <c r="G9" s="1">
         <v>10</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>20</v>
@@ -1586,39 +1653,36 @@
         <v>20</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>129</v>
+        <v>166</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="O9" s="1">
         <v>2023</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>131</v>
+        <v>169</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>63</v>
@@ -1627,19 +1691,16 @@
         <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>1000000</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
+        <v>426000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>20</v>
@@ -1648,13 +1709,16 @@
         <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>122</v>
+        <v>20</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="O10" s="1">
         <v>2023</v>
@@ -1663,21 +1727,24 @@
         <v>67</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>120</v>
+        <v>158</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>55</v>
+        <v>160</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
@@ -1686,308 +1753,314 @@
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5">
+        <v>87540</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="O11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>170</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2">
         <f>121839+34057</f>
         <v>155896</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F14" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="12" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O14" s="1">
         <v>2023</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3030000</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="1">
-        <v>34</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="O12" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="2">
-        <v>26712</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>641</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="O13" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3000000</v>
-      </c>
-      <c r="G14" s="1">
-        <v>27</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="O14" s="1">
-        <v>2022</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R14" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2">
-        <v>230000</v>
+        <v>3030000</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="G15" s="1">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="O15" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2">
-        <v>571645</v>
+        <v>26712</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
-        <v>8</v>
+        <v>641</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
@@ -2001,28 +2074,31 @@
       <c r="L16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="14" t="s">
-        <v>107</v>
+      <c r="M16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="O16" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -2031,134 +2107,120 @@
         <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>103462</v>
-      </c>
-      <c r="F17" s="1">
-        <v>5</v>
+        <v>2400000</v>
       </c>
       <c r="G17" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" s="1">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>76</v>
+        <v>20</v>
+      </c>
+      <c r="N17" t="s">
+        <v>211</v>
       </c>
       <c r="O17" s="1">
-        <v>2021</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>164</v>
-      </c>
+        <v>2022</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="G18" s="1">
         <v>27</v>
       </c>
-      <c r="E18" s="2">
-        <v>582000</v>
-      </c>
-      <c r="F18" s="1">
-        <v>8</v>
-      </c>
-      <c r="G18" s="1">
-        <v>10</v>
-      </c>
       <c r="H18" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>59</v>
+        <v>184</v>
       </c>
       <c r="O18" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="R18" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="5">
-        <v>2100000</v>
+        <v>27</v>
+      </c>
+      <c r="E19" s="2">
+        <v>230000</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="G19" s="1">
-        <v>10</v>
-      </c>
-      <c r="H19" s="1">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>20</v>
@@ -2173,33 +2235,30 @@
         <v>20</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="O19" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2208,17 +2267,20 @@
         <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="5">
-        <v>860304</v>
-      </c>
-      <c r="F20" s="1">
+        <v>27</v>
+      </c>
+      <c r="E20" s="2">
+        <v>571645</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1">
         <v>8</v>
       </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
       <c r="I20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2226,39 +2288,36 @@
         <v>20</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>176</v>
+        <v>20</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="O20" s="1">
         <v>2021</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q20" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="R20" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -2270,16 +2329,16 @@
         <v>26</v>
       </c>
       <c r="E21" s="2">
-        <v>2700000</v>
+        <v>103462</v>
       </c>
       <c r="F21" s="1">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>20</v>
@@ -2288,54 +2347,57 @@
         <v>21</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="O21" s="1">
-        <v>2020</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>39</v>
+        <v>2021</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="T21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="E22" s="2">
+        <v>582000</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1">
+        <v>10</v>
       </c>
       <c r="H22" s="1">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>20</v>
@@ -2344,36 +2406,33 @@
         <v>20</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>92</v>
+      <c r="N22" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="O22" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>91</v>
+        <v>60</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -2382,19 +2441,16 @@
         <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="5">
-        <v>2900000</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="1">
-        <v>50</v>
+        <v>860304</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8</v>
       </c>
       <c r="H23" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>20</v>
@@ -2403,36 +2459,39 @@
         <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>105</v>
+        <v>175</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="O23" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>106</v>
+        <v>174</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="T23" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
@@ -2444,16 +2503,16 @@
         <v>26</v>
       </c>
       <c r="E24" s="2">
-        <v>77558</v>
+        <v>2700000</v>
       </c>
       <c r="F24" s="1">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="G24" s="1">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H24" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>20</v>
@@ -2462,55 +2521,55 @@
         <v>21</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="O24" s="1">
         <v>2020</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1">
         <v>58</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="5">
-        <v>37000</v>
-      </c>
-      <c r="F25" s="1">
-        <v>8</v>
-      </c>
-      <c r="G25" s="1">
-        <v>32</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
       <c r="I25" s="1" t="s">
         <v>20</v>
       </c>
@@ -2518,36 +2577,39 @@
         <v>20</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N25" s="7" t="s">
-        <v>77</v>
+        <v>20</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="O25" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R25" s="6" t="s">
-        <v>79</v>
+        <v>93</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>20</v>
@@ -2555,17 +2617,14 @@
       <c r="D26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="5">
-        <v>21000</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
+      <c r="E26" s="2">
+        <v>1600000</v>
+      </c>
+      <c r="G26" s="1">
+        <v>10</v>
       </c>
       <c r="H26" s="1">
-        <v>2772</v>
+        <v>51</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>20</v>
@@ -2579,52 +2638,58 @@
       <c r="L26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N26" s="7" t="s">
-        <v>86</v>
+      <c r="M26" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="O26" s="1">
-        <v>2019</v>
+        <v>2020</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>88</v>
+        <v>214</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>212</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>89</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="2">
-        <v>105459</v>
+      <c r="E27" s="5">
+        <v>2900000</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G27" s="1">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="H27" s="1">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>20</v>
@@ -2633,155 +2698,379 @@
         <v>20</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="O27" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="P27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="2">
+        <v>77558</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2020</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="R27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="Q28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
-        <v>146</v>
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="5">
+        <v>37000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1">
+        <v>32</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2019</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="5">
+        <v>21000</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2772</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="2">
+        <v>105459</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A34" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E34" s="2">
         <f>490000*6</f>
         <v>2940000</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F34" s="1">
         <v>4</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G34" s="1">
         <v>36</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H34" s="1">
         <v>0</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="I34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N30" s="7" t="s">
+      <c r="N34" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O34" s="1">
         <v>2022</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="R34" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="T30" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A35" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G35" s="1">
         <v>931</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H35" s="1">
         <v>4336</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="1" t="s">
+      <c r="I35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N31" s="7" t="s">
+      <c r="N35" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O35" s="1">
         <v>2021</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="R31" s="15" t="s">
+      <c r="R35" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="T31" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F14:H14"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:M1"/>
@@ -2794,31 +3083,34 @@
   <hyperlinks>
     <hyperlink ref="R3" r:id="rId1" location="both57m-dataset" xr:uid="{6093CB3F-7559-4A60-9533-FC5A6593C8DF}"/>
     <hyperlink ref="R4" r:id="rId2" display="https://hograspnet2024.github.io/" xr:uid="{DF9465E4-05AF-4DCB-BCDC-1DC144B7533F}"/>
-    <hyperlink ref="R19" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
-    <hyperlink ref="R12" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
-    <hyperlink ref="R18" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
-    <hyperlink ref="R13" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
-    <hyperlink ref="R24" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
-    <hyperlink ref="R17" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
-    <hyperlink ref="R25" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
-    <hyperlink ref="R26" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
-    <hyperlink ref="R22" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
-    <hyperlink ref="R27" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
-    <hyperlink ref="R23" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
-    <hyperlink ref="R16" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
-    <hyperlink ref="R15" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
-    <hyperlink ref="R10" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
-    <hyperlink ref="R21" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
-    <hyperlink ref="R9" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
-    <hyperlink ref="R11" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
-    <hyperlink ref="R31" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
-    <hyperlink ref="R8" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
-    <hyperlink ref="R7" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
-    <hyperlink ref="R20" r:id="rId23" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/HanCo.en.html" xr:uid="{1D766960-F6F8-4DD4-BE6E-EE217414AB48}"/>
-    <hyperlink ref="R5" r:id="rId24" display="https://tars-home.github.io/hohdataset/" xr:uid="{9D883F19-E811-4E4A-8132-DA3D28491038}"/>
-    <hyperlink ref="R14" r:id="rId25" display="https://menghao666.github.io/HDR/" xr:uid="{CC6BDE28-D08F-4D4E-BC32-67420002F467}"/>
+    <hyperlink ref="R8" r:id="rId3" display="https://arctic.is.tue.mpg.de./" xr:uid="{67C70230-F66A-4B58-B908-BAA69BCE285D}"/>
+    <hyperlink ref="R15" r:id="rId4" location="dataset-preparation" display="https://github.com/facebookresearch/assemblyhands-toolkit?tab=readme-ov-file - dataset-preparation" xr:uid="{BA994E02-7C9A-480C-9BE7-469C80CFF2D3}"/>
+    <hyperlink ref="R22" r:id="rId5" xr:uid="{24D50E73-BE3C-4D59-802D-FC5B0F458535}"/>
+    <hyperlink ref="R16" r:id="rId6" xr:uid="{A385A040-B124-451A-B75D-B33F24772B9F}"/>
+    <hyperlink ref="R28" r:id="rId7" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{4995C41F-00B3-4BCD-99A4-6C0737AD5616}"/>
+    <hyperlink ref="R21" r:id="rId8" display="https://www.tugraz.at/index.php?id=40231" xr:uid="{373D98B6-08E8-42E7-A346-A5029019BE25}"/>
+    <hyperlink ref="R29" r:id="rId9" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/FreihandDataset.en.html" xr:uid="{6672DE66-0A0F-4B20-B684-4ACBEA43D846}"/>
+    <hyperlink ref="R30" r:id="rId10" display="https://www.di.ens.fr/willow/research/obman/data/" xr:uid="{4AA12478-23BE-477D-90C4-DD7FA985BDA4}"/>
+    <hyperlink ref="R25" r:id="rId11" xr:uid="{5528656B-F525-4E0E-9AB0-6BEFB18482F4}"/>
+    <hyperlink ref="R31" r:id="rId12" display="https://github.com/guiggh/hand_pose_action" xr:uid="{A91A1197-D35A-4C81-B0F5-E0D689528F42}"/>
+    <hyperlink ref="R27" r:id="rId13" display="https://ieee-dataport.org/documents/contactpose-part-1" xr:uid="{A12604FD-8B35-4A81-BAA0-D3910A5BDB54}"/>
+    <hyperlink ref="R20" r:id="rId14" display="https://h2odataset.ethz.ch/" xr:uid="{96107C85-5C37-48BF-A931-71FBADA5759C}"/>
+    <hyperlink ref="R19" r:id="rId15" display="https://oakink.net/" xr:uid="{73A78462-4851-45B6-B748-0A6E94663EDD}"/>
+    <hyperlink ref="R13" r:id="rId16" xr:uid="{7C1FE143-B5CC-4BF6-999A-CC5FC5FE2101}"/>
+    <hyperlink ref="R24" r:id="rId17" display="https://mks0601.github.io/InterHand2.6M/" xr:uid="{3F0A2960-E8A9-49D2-82A6-46A79ECB732B}"/>
+    <hyperlink ref="R12" r:id="rId18" display="https://mks0601.github.io/ReInterHand/" xr:uid="{5A93AB77-20BF-4471-803D-2BAB9880B54F}"/>
+    <hyperlink ref="R14" r:id="rId19" xr:uid="{ED115BC3-A0DF-4B37-9B77-88F8F35C8F5C}"/>
+    <hyperlink ref="R35" r:id="rId20" display="https://ego4d-data.org/" xr:uid="{CFA360B3-53BF-4344-9586-627AFE18D022}"/>
+    <hyperlink ref="R11" r:id="rId21" display="https://europe.naverlabs.com/research/showme/" xr:uid="{F94534C3-BA4B-4302-8C05-64052BC2A341}"/>
+    <hyperlink ref="R10" r:id="rId22" xr:uid="{AD425495-D8EE-47D1-9E1E-D61340901745}"/>
+    <hyperlink ref="R23" r:id="rId23" display="https://lmb.informatik.uni-freiburg.de/resources/datasets/HanCo.en.html" xr:uid="{1D766960-F6F8-4DD4-BE6E-EE217414AB48}"/>
+    <hyperlink ref="R7" r:id="rId24" display="https://tars-home.github.io/hohdataset/" xr:uid="{9D883F19-E811-4E4A-8132-DA3D28491038}"/>
+    <hyperlink ref="R18" r:id="rId25" display="https://menghao666.github.io/HDR/" xr:uid="{CC6BDE28-D08F-4D4E-BC32-67420002F467}"/>
+    <hyperlink ref="R6" r:id="rId26" display="https://oakink.net/v2/" xr:uid="{EC0ABD21-C3C8-4506-915C-3C580E463179}"/>
+    <hyperlink ref="R5" r:id="rId27" display="https://taco2024.github.io/" xr:uid="{78294359-D9AE-4AF8-A2B6-31F219DDF2AE}"/>
+    <hyperlink ref="R26" r:id="rId28" display="https://grab.is.tue.mpg.de/" xr:uid="{36D8EEB2-4691-42E2-8C84-9DDEEF7E23E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>